<commit_message>
TS Kramam 7.4, TS Template files 08/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302FC03F-7EAC-4375-999A-5E019ED2090B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243C1D98-6459-4DCE-A298-45B87CBC0753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="69">
   <si>
     <t>Srl No</t>
   </si>
@@ -246,13 +246,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -327,22 +333,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -632,7 +639,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,16 +670,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="7" t="s">
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -761,13 +768,27 @@
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="C5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J5" s="4" t="s">
         <v>68</v>
       </c>
@@ -777,7 +798,9 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="O5" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -798,13 +821,27 @@
       <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="C6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J6" s="4" t="s">
         <v>68</v>
       </c>
@@ -814,7 +851,9 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="O6" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -835,13 +874,27 @@
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="C7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J7" s="4" t="s">
         <v>68</v>
       </c>
@@ -851,7 +904,9 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="O7" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -872,13 +927,27 @@
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="C8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J8" s="4" t="s">
         <v>68</v>
       </c>
@@ -888,7 +957,9 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="O8" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -909,13 +980,27 @@
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="C9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J9" s="4" t="s">
         <v>68</v>
       </c>
@@ -925,7 +1010,9 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -946,13 +1033,27 @@
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="C10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>68</v>
       </c>
@@ -962,7 +1063,9 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="O10" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -983,13 +1086,27 @@
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="C11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J11" s="4" t="s">
         <v>68</v>
       </c>
@@ -999,7 +1116,9 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="O11" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -1020,13 +1139,27 @@
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="C12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J12" s="4" t="s">
         <v>68</v>
       </c>
@@ -1036,7 +1169,9 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+      <c r="O12" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -1057,9 +1192,15 @@
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1073,7 +1214,9 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+      <c r="O13" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -1094,9 +1237,15 @@
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="C14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1110,7 +1259,9 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="O14" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -1131,12 +1282,20 @@
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
         <v>68</v>
@@ -1168,9 +1327,15 @@
       <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="C16" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -1201,9 +1366,15 @@
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -1234,9 +1405,15 @@
       <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1267,16 +1444,22 @@
       <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="9" t="s">
+      <c r="C19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F19" s="6">
         <v>44656</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1304,12 +1487,20 @@
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1337,9 +1528,15 @@
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="C21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1370,9 +1567,15 @@
       <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="C22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1403,9 +1606,15 @@
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="C23" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1436,8 +1645,12 @@
       <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="C24" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E24" s="4" t="s">
         <v>68</v>
       </c>
@@ -1473,8 +1686,12 @@
       <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="C25" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E25" s="4" t="s">
         <v>68</v>
       </c>
@@ -1510,8 +1727,12 @@
       <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="C26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1543,8 +1764,12 @@
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -1576,8 +1801,12 @@
       <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="C28" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1609,8 +1838,12 @@
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="C29" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -1642,8 +1875,12 @@
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="C30" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1675,8 +1912,12 @@
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="C31" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1708,8 +1949,12 @@
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
+      <c r="C32" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1741,8 +1986,12 @@
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="C33" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1774,8 +2023,12 @@
       <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="C34" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1807,8 +2060,12 @@
       <c r="B35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="C35" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1840,8 +2097,12 @@
       <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+      <c r="C36" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1873,8 +2134,12 @@
       <c r="B37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="C37" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -1906,8 +2171,12 @@
       <c r="B38" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="C38" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1939,8 +2208,12 @@
       <c r="B39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -1972,8 +2245,12 @@
       <c r="B40" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="C40" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2005,8 +2282,12 @@
       <c r="B41" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -2038,8 +2319,12 @@
       <c r="B42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="C42" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2071,8 +2356,12 @@
       <c r="B43" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2104,8 +2393,12 @@
       <c r="B44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
+      <c r="C44" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2137,8 +2430,12 @@
       <c r="B45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+      <c r="C45" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2170,8 +2467,12 @@
       <c r="B46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+      <c r="C46" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -2203,8 +2504,12 @@
       <c r="B47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="C47" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -2236,8 +2541,12 @@
       <c r="B48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
+      <c r="C48" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -7533,7 +7842,7 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS 7.1 Tamil Kramam and TS 3.2 heard Excel updated - 08/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243C1D98-6459-4DCE-A298-45B87CBC0753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271FB749-CCB0-43BE-8654-050082242D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,13 +346,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,7 +639,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,16 +670,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="8" t="s">
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -768,25 +768,25 @@
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="10" t="s">
+      <c r="C5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -798,7 +798,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P5" s="4"/>
@@ -821,25 +821,25 @@
       <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -851,7 +851,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P6" s="4"/>
@@ -874,25 +874,25 @@
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="10" t="s">
+      <c r="C7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J7" s="4" t="s">
@@ -904,7 +904,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P7" s="4"/>
@@ -927,25 +927,25 @@
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="10" t="s">
+      <c r="C8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -957,7 +957,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P8" s="4"/>
@@ -980,25 +980,25 @@
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="10" t="s">
+      <c r="C9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J9" s="4" t="s">
@@ -1010,7 +1010,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="10" t="s">
+      <c r="O9" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P9" s="4"/>
@@ -1033,25 +1033,25 @@
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="10" t="s">
+      <c r="C10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -1063,7 +1063,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P10" s="4"/>
@@ -1086,25 +1086,25 @@
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="10" t="s">
+      <c r="C11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J11" s="4" t="s">
@@ -1116,7 +1116,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P11" s="4"/>
@@ -1139,25 +1139,25 @@
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="C12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>68</v>
       </c>
       <c r="J12" s="4" t="s">
@@ -1169,7 +1169,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="10" t="s">
+      <c r="O12" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P12" s="4"/>
@@ -1192,13 +1192,13 @@
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="C13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F13" s="4"/>
@@ -1214,7 +1214,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="10" t="s">
+      <c r="O13" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P13" s="4"/>
@@ -1237,13 +1237,13 @@
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="C14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F14" s="4"/>
@@ -1259,7 +1259,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="10" t="s">
+      <c r="O14" s="8" t="s">
         <v>68</v>
       </c>
       <c r="P14" s="4"/>
@@ -1282,18 +1282,18 @@
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I15" s="4"/>
@@ -1327,13 +1327,13 @@
       <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="C16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F16" s="4"/>
@@ -1366,13 +1366,13 @@
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="C17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F17" s="4"/>
@@ -1405,13 +1405,13 @@
       <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="C18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F18" s="4"/>
@@ -1444,10 +1444,10 @@
       <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="C19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -1457,7 +1457,7 @@
         <v>44656</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I19" s="4"/>
@@ -1487,18 +1487,20 @@
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="6">
+        <v>44659</v>
+      </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I20" s="4"/>
@@ -1528,10 +1530,10 @@
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -1567,10 +1569,10 @@
       <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E22" s="7" t="s">
@@ -1606,10 +1608,10 @@
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -1645,10 +1647,10 @@
       <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -1686,10 +1688,10 @@
       <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -1727,10 +1729,10 @@
       <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E26" s="4"/>
@@ -1764,10 +1766,10 @@
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="C27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E27" s="4"/>
@@ -1801,10 +1803,10 @@
       <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="C28" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E28" s="4"/>
@@ -1838,10 +1840,10 @@
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E29" s="4"/>
@@ -1875,10 +1877,10 @@
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="C30" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E30" s="4"/>
@@ -1912,10 +1914,10 @@
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="C31" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E31" s="4"/>
@@ -1949,10 +1951,10 @@
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="C32" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E32" s="4"/>
@@ -1986,10 +1988,10 @@
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="C33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E33" s="4"/>
@@ -2023,10 +2025,10 @@
       <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="C34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="4"/>
@@ -2060,10 +2062,10 @@
       <c r="B35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="10" t="s">
+      <c r="C35" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="4"/>
@@ -2097,10 +2099,10 @@
       <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="C36" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="4"/>
@@ -2134,10 +2136,10 @@
       <c r="B37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="10" t="s">
+      <c r="C37" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="4"/>
@@ -2171,10 +2173,10 @@
       <c r="B38" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="C38" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E38" s="4"/>
@@ -2208,10 +2210,10 @@
       <c r="B39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="10" t="s">
+      <c r="C39" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E39" s="4"/>
@@ -2245,10 +2247,10 @@
       <c r="B40" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="C40" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E40" s="4"/>
@@ -2282,10 +2284,10 @@
       <c r="B41" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="10" t="s">
+      <c r="C41" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E41" s="4"/>
@@ -2319,10 +2321,10 @@
       <c r="B42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="C42" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E42" s="4"/>
@@ -2356,10 +2358,10 @@
       <c r="B43" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="10" t="s">
+      <c r="C43" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E43" s="4"/>
@@ -2393,10 +2395,10 @@
       <c r="B44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="10" t="s">
+      <c r="C44" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E44" s="4"/>
@@ -2430,10 +2432,10 @@
       <c r="B45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" s="10" t="s">
+      <c r="C45" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E45" s="4"/>
@@ -2467,10 +2469,10 @@
       <c r="B46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="10" t="s">
+      <c r="C46" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E46" s="4"/>
@@ -2504,10 +2506,10 @@
       <c r="B47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" s="10" t="s">
+      <c r="C47" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E47" s="4"/>
@@ -2541,10 +2543,10 @@
       <c r="B48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" s="10" t="s">
+      <c r="C48" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E48" s="4"/>

</xml_diff>

<commit_message>
TS 3.2, 3.3 Template After Ghanam hearing - 10/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271FB749-CCB0-43BE-8654-050082242D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77D3281-2918-41E4-81DB-89FB76D000CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="69">
   <si>
     <t>Srl No</t>
   </si>
@@ -639,7 +639,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1202,9 @@
         <v>68</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
@@ -1247,7 +1249,9 @@
         <v>68</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
@@ -1539,7 +1543,9 @@
       <c r="E21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="6">
+        <v>44661</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -1809,12 +1815,22 @@
       <c r="D28" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -1883,12 +1899,22 @@
       <c r="D30" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>

</xml_diff>

<commit_message>
Update to Jatai Ghanam Status
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77D3281-2918-41E4-81DB-89FB76D000CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F37F01-5BB5-455D-8437-578BC9264552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="69">
   <si>
     <t>Srl No</t>
   </si>
@@ -246,13 +246,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -333,26 +339,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,7 +646,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1471,9 @@
       <c r="H19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -1507,7 +1516,9 @@
       <c r="H20" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -1547,8 +1558,12 @@
         <v>44661</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="H21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
@@ -7870,7 +7885,7 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS Ghanam Status Padam Templates TS3.4 and 3.5 12/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F37F01-5BB5-455D-8437-578BC9264552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5086BFB5-274B-409D-BB3E-E1B407BE2B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="69">
   <si>
     <t>Srl No</t>
   </si>
@@ -246,13 +246,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -339,27 +345,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,10 +650,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,16 +684,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="9" t="s">
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1212,8 +1219,12 @@
       <c r="G13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="H13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="J13" s="4" t="s">
         <v>68</v>
       </c>
@@ -1259,8 +1270,12 @@
       <c r="G14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="H14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="J14" s="4" t="s">
         <v>68</v>
       </c>
@@ -1471,7 +1486,7 @@
       <c r="H19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="9" t="s">
         <v>68</v>
       </c>
       <c r="J19" s="4"/>
@@ -1516,7 +1531,7 @@
       <c r="H20" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="9" t="s">
         <v>68</v>
       </c>
       <c r="J20" s="4"/>
@@ -1561,7 +1576,7 @@
       <c r="H21" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="9" t="s">
         <v>68</v>
       </c>
       <c r="J21" s="4"/>
@@ -1601,8 +1616,12 @@
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="H22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
@@ -1640,8 +1659,12 @@
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="H23" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -7885,7 +7908,7 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS 3.4 Template after hearing - 13/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5086BFB5-274B-409D-BB3E-E1B407BE2B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6016FCCA-1571-4FFA-A790-4891074F502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,10 +650,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,7 +1614,9 @@
       <c r="E22" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="6">
+        <v>44664</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="10" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
TS Templates and Dheerga Swaritam - 15/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6016FCCA-1571-4FFA-A790-4891074F502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FBD5B7-BCDE-428C-8468-3FC3D8F9113E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,10 +650,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1659,9 @@
       <c r="E23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="6">
+        <v>44665</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="10" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
TS 4.3 Template after hearing - 16/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FBD5B7-BCDE-428C-8468-3FC3D8F9113E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B24E28C-F564-4CC2-B0CB-5B9BD668CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="70">
   <si>
     <t>Srl No</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>TTD Jatai Hearing 1</t>
-  </si>
-  <si>
-    <t>Ghanam Hearing</t>
   </si>
   <si>
     <t>Basic Checks</t>
@@ -240,6 +237,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Ghanam Hearing 1</t>
+  </si>
+  <si>
+    <t>Ghanam Hearing Final</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,12 +688,12 @@
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="U2" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
       <c r="X2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
@@ -706,73 +709,73 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="U3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="X3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="18" x14ac:dyDescent="0.25">
@@ -780,40 +783,40 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -833,40 +836,40 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -886,40 +889,40 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -939,40 +942,40 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -992,40 +995,40 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -1045,40 +1048,40 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1098,40 +1101,40 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -1151,40 +1154,40 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -1204,38 +1207,38 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -1255,38 +1258,38 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
@@ -1306,28 +1309,28 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -1351,16 +1354,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1390,16 +1393,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1429,16 +1432,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1468,26 +1471,26 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" s="6">
         <v>44656</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1513,26 +1516,26 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F20" s="6">
         <v>44659</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1558,26 +1561,26 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F21" s="6">
         <v>44661</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1603,26 +1606,26 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" s="6">
         <v>44664</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1648,26 +1651,26 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" s="6">
         <v>44665</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1693,16 +1696,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F24" s="6">
         <v>44649</v>
@@ -1734,16 +1737,16 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F25" s="6">
         <v>44652</v>
@@ -1775,16 +1778,20 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="6">
+        <v>44667</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -1812,15 +1819,17 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1849,29 +1858,29 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1896,13 +1905,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1933,29 +1942,29 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -1980,13 +1989,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2017,13 +2026,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2054,13 +2063,13 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2091,13 +2100,13 @@
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2128,13 +2137,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2165,13 +2174,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2202,13 +2211,13 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -2239,13 +2248,13 @@
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2276,13 +2285,13 @@
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -2313,13 +2322,13 @@
         <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -2350,13 +2359,13 @@
         <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -2387,13 +2396,13 @@
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2424,13 +2433,13 @@
         <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -2461,13 +2470,13 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2498,13 +2507,13 @@
         <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -2535,13 +2544,13 @@
         <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -2572,13 +2581,13 @@
         <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -2609,13 +2618,13 @@
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>

</xml_diff>

<commit_message>
Jatai Ghanam Status file -16/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B24E28C-F564-4CC2-B0CB-5B9BD668CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B1BF79-34A6-4DB4-A80E-92868A4B670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="70">
   <si>
     <t>Srl No</t>
   </si>
@@ -656,7 +656,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,11 +679,9 @@
     <col min="18" max="18" width="14.28515625" customWidth="1"/>
     <col min="19" max="19" width="14.85546875" customWidth="1"/>
     <col min="20" max="20" width="13.28515625" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" customWidth="1"/>
+    <col min="23" max="26" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
@@ -1234,9 +1232,15 @@
       <c r="K13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="L13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="O13" s="8" t="s">
         <v>67</v>
       </c>
@@ -1245,12 +1249,24 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="5"/>
+      <c r="U13" s="6">
+        <v>44649</v>
+      </c>
+      <c r="V13" s="6">
+        <v>44649</v>
+      </c>
+      <c r="W13" s="6">
+        <v>44650</v>
+      </c>
+      <c r="X13" s="6">
+        <v>44649</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>44649</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>44650</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1285,22 +1301,44 @@
       <c r="K14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="L14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="O14" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
+      <c r="P14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
+      <c r="U14" s="6">
+        <v>44667</v>
+      </c>
+      <c r="V14" s="6">
+        <v>44667</v>
+      </c>
       <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
+      <c r="X14" s="6">
+        <v>44667</v>
+      </c>
+      <c r="Y14" s="6">
+        <v>44667</v>
+      </c>
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TS 2.4 editing and TS 4.4 hearing - 18/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B1BF79-34A6-4DB4-A80E-92868A4B670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14E4D4C-9EAF-49DC-8479-E225929EB5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,13 +249,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -348,28 +354,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +663,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
+      <selection pane="bottomRight" activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,14 +1339,18 @@
       <c r="V14" s="6">
         <v>44667</v>
       </c>
-      <c r="W14" s="4"/>
+      <c r="W14" s="13">
+        <v>44668</v>
+      </c>
       <c r="X14" s="6">
         <v>44667</v>
       </c>
       <c r="Y14" s="6">
         <v>44667</v>
       </c>
-      <c r="Z14" s="5"/>
+      <c r="Z14" s="13">
+        <v>44668</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -7959,7 +7970,7 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Ghanam Hearing TS 4.4,4.6 and template 2.4 - 20/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14E4D4C-9EAF-49DC-8479-E225929EB5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A707A06C-17C6-4838-8030-01A199DEF5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="70">
   <si>
     <t>Srl No</t>
   </si>
@@ -370,13 +370,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +660,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z14" sqref="Z14"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,16 +692,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="U2" s="11" t="s">
+      <c r="U2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="11" t="s">
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1339,7 +1339,7 @@
       <c r="V14" s="6">
         <v>44667</v>
       </c>
-      <c r="W14" s="13">
+      <c r="W14" s="11">
         <v>44668</v>
       </c>
       <c r="X14" s="6">
@@ -1348,7 +1348,7 @@
       <c r="Y14" s="6">
         <v>44667</v>
       </c>
-      <c r="Z14" s="13">
+      <c r="Z14" s="11">
         <v>44668</v>
       </c>
     </row>
@@ -1370,11 +1370,15 @@
         <v>67</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="J15" s="4" t="s">
         <v>67</v>
       </c>
@@ -1879,7 +1883,9 @@
       <c r="E27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="6">
+        <v>44669</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1962,8 +1968,12 @@
       <c r="D29" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="6">
+        <v>44671</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>

</xml_diff>

<commit_message>
TS 5.1 Archieve listening update - 28/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A707A06C-17C6-4838-8030-01A199DEF5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A9B712-BD90-427E-A9A6-C56020343FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="70">
   <si>
     <t>Srl No</t>
   </si>
@@ -660,10 +660,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,14 +671,14 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
     <col min="15" max="15" width="13.140625" customWidth="1"/>
     <col min="16" max="16" width="18.140625" customWidth="1"/>
@@ -1385,8 +1385,12 @@
       <c r="K15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="L15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="6">
+        <v>44674</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -1419,7 +1423,9 @@
         <v>67</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1458,7 +1464,9 @@
         <v>67</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1497,7 +1505,9 @@
         <v>67</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1538,7 +1548,9 @@
       <c r="F19" s="6">
         <v>44656</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H19" s="8" t="s">
         <v>67</v>
       </c>
@@ -1583,7 +1595,9 @@
       <c r="F20" s="6">
         <v>44659</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H20" s="8" t="s">
         <v>67</v>
       </c>
@@ -1628,7 +1642,9 @@
       <c r="F21" s="6">
         <v>44661</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H21" s="8" t="s">
         <v>67</v>
       </c>
@@ -1673,7 +1689,9 @@
       <c r="F22" s="6">
         <v>44664</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H22" s="10" t="s">
         <v>67</v>
       </c>
@@ -1718,7 +1736,9 @@
       <c r="F23" s="6">
         <v>44665</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H23" s="10" t="s">
         <v>67</v>
       </c>
@@ -1763,7 +1783,9 @@
       <c r="F24" s="6">
         <v>44649</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1804,7 +1826,9 @@
       <c r="F25" s="6">
         <v>44652</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1845,7 +1869,9 @@
       <c r="F26" s="6">
         <v>44667</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1886,7 +1912,9 @@
       <c r="F27" s="6">
         <v>44669</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1927,7 +1955,9 @@
       <c r="F28" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="4"/>
+      <c r="G28" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H28" s="4" t="s">
         <v>67</v>
       </c>
@@ -1974,7 +2004,9 @@
       <c r="F29" s="6">
         <v>44671</v>
       </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -2015,7 +2047,9 @@
       <c r="F30" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="H30" s="4" t="s">
         <v>67</v>
       </c>
@@ -2056,11 +2090,15 @@
       <c r="D31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="6">
+        <v>44678</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>

</xml_diff>

<commit_message>
TS 5.1afte archive hearing -Status update - 30/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A9B712-BD90-427E-A9A6-C56020343FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF95E6-F0E2-48E0-A0E1-D47723F738B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,10 +660,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2093,9 @@
       <c r="E31" s="6">
         <v>44678</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="6">
+        <v>44681</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">

</xml_diff>

<commit_message>
Jatai TS 5.2 heard TTD - 04/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF95E6-F0E2-48E0-A0E1-D47723F738B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D420E4-BD27-4033-9180-C0A424ADFF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,7 +663,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2133,9 @@
       <c r="D32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="6">
+        <v>44685</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>

</xml_diff>

<commit_message>
TS 5.2 Ghanam Hearing and edits - 05/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D420E4-BD27-4033-9180-C0A424ADFF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1970699F-27A7-4A17-97C7-3AA6F3995979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,7 +663,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2136,9 @@
       <c r="E32" s="6">
         <v>44685</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="6">
+        <v>44686</v>
+      </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>

</xml_diff>

<commit_message>
TS 5.3 Jatai TTD heard - 06/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1970699F-27A7-4A17-97C7-3AA6F3995979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFC24D6-A723-4F51-81DC-3B539E31FF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,10 +660,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,7 +2174,9 @@
       <c r="D33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="6">
+        <v>44687</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>

</xml_diff>

<commit_message>
TS 5.4 Jatai TTD Heard - 08/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFC24D6-A723-4F51-81DC-3B539E31FF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC362AC-DF42-4CF9-9055-D3FD25FD1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,10 +660,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,7 +2213,9 @@
       <c r="D34" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="6">
+        <v>44689</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>

</xml_diff>

<commit_message>
TS 5.7 Template TTD Hearing - 11/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC362AC-DF42-4CF9-9055-D3FD25FD1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ED967F-01B5-4A08-A260-DCABD9F50E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,7 +663,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,7 +2252,9 @@
       <c r="D35" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="6">
+        <v>44690</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -2289,7 +2291,9 @@
       <c r="D36" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="6">
+        <v>44691</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -2326,7 +2330,9 @@
       <c r="D37" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="6">
+        <v>44692</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>

</xml_diff>

<commit_message>
TS 2.4 Template with 1 correction -13/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ED967F-01B5-4A08-A260-DCABD9F50E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACBCE2A-AAAB-40B1-96DC-11599F10E776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="70">
   <si>
     <t>Srl No</t>
   </si>
@@ -663,7 +663,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,16 +1317,16 @@
       <c r="N14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="O14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="R14" s="8" t="s">
+      <c r="O14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" s="4" t="s">
         <v>67</v>
       </c>
       <c r="S14" s="8" t="s">
@@ -1391,19 +1391,43 @@
       <c r="M15" s="6">
         <v>44674</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="5"/>
+      <c r="U15" s="6">
+        <v>44691</v>
+      </c>
+      <c r="V15" s="6">
+        <v>44691</v>
+      </c>
+      <c r="W15" s="6">
+        <v>44692</v>
+      </c>
+      <c r="X15" s="6">
+        <v>44693</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>44693</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>44693</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">

</xml_diff>

<commit_message>
TS 2.4 Raja Input Baraha for Ghanam and Jatai - 15/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACBCE2A-AAAB-40B1-96DC-11599F10E776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FDD15E-FE87-48D4-BB7F-242F18AF49E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,7 +663,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,7 +2201,9 @@
       <c r="E33" s="6">
         <v>44687</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="6">
+        <v>44696</v>
+      </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>

</xml_diff>

<commit_message>
GS 1.1-1.8 Reviewed and Pushed - 19/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FDD15E-FE87-48D4-BB7F-242F18AF49E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D12237D-F535-4AAB-9E3A-D17D697AF083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="70">
   <si>
     <t>Srl No</t>
   </si>
@@ -249,13 +249,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -354,29 +360,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +667,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,12 +1457,24 @@
       <c r="G16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="H16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" s="6">
+        <v>44697</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -2242,7 +2261,9 @@
       <c r="E34" s="6">
         <v>44689</v>
       </c>
-      <c r="F34" s="4"/>
+      <c r="F34" s="6">
+        <v>44699</v>
+      </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -8060,7 +8081,7 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS 5.5 - 5.7 Template - Ghanam hearing till 5.7
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D12237D-F535-4AAB-9E3A-D17D697AF083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F07670-54C2-4A0D-910A-AB392FE0770F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,13 +249,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -360,30 +366,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,10 +674,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,16 +706,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="12" t="s">
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1457,19 +1464,19 @@
       <c r="G16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="L16" s="14" t="s">
+      <c r="H16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>67</v>
       </c>
       <c r="M16" s="6">
@@ -2302,7 +2309,9 @@
       <c r="E35" s="6">
         <v>44690</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="13">
+        <v>44701</v>
+      </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -2341,7 +2350,9 @@
       <c r="E36" s="6">
         <v>44691</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F36" s="6">
+        <v>44703</v>
+      </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -2380,7 +2391,9 @@
       <c r="E37" s="6">
         <v>44692</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="6">
+        <v>44704</v>
+      </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -8081,7 +8094,7 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS 2.4 Ghanam Tamil - 01-06-2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F07670-54C2-4A0D-910A-AB392FE0770F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C6C90A-9292-4429-B251-AE2FF911ED06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="70">
   <si>
     <t>Srl No</t>
   </si>
@@ -249,13 +249,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -366,31 +372,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,10 +681,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,16 +1489,34 @@
       <c r="M16" s="6">
         <v>44697</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
+      <c r="N16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
+      <c r="U16" s="6">
+        <v>44713</v>
+      </c>
+      <c r="V16" s="6">
+        <v>44713</v>
+      </c>
+      <c r="W16" s="6">
+        <v>44713</v>
+      </c>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
       <c r="Z16" s="5"/>
@@ -8094,7 +8119,7 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS Ghanam Jatai Status
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
+++ b/TS Jatai Ghanam Project/TS Jatai Ghanam Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C6C90A-9292-4429-B251-AE2FF911ED06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC979D4-912C-4B23-9F9F-25348EFABCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,13 +391,13 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,10 +681,10 @@
   <dimension ref="A2:Z243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X16" sqref="X16"/>
+      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,16 +713,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="14" t="s">
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1489,22 +1489,22 @@
       <c r="M16" s="6">
         <v>44697</v>
       </c>
-      <c r="N16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="P16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="R16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="S16" s="16" t="s">
+      <c r="N16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="14" t="s">
         <v>67</v>
       </c>
       <c r="T16" s="4"/>
@@ -1517,9 +1517,15 @@
       <c r="W16" s="6">
         <v>44713</v>
       </c>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="5"/>
+      <c r="X16" s="6">
+        <v>44714</v>
+      </c>
+      <c r="Y16" s="6">
+        <v>44714</v>
+      </c>
+      <c r="Z16" s="6">
+        <v>44715</v>
+      </c>
     </row>
     <row r="17" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">

</xml_diff>